<commit_message>
revisi: adding ipk semester
</commit_message>
<xml_diff>
--- a/assets/document/data-latih/Book8.xlsx
+++ b/assets/document/data-latih/Book8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arlan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1274D987-E676-4B1F-A03E-A3F74884608C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{17144A63-B04E-4207-8B6B-9840CB48F91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26475" yWindow="-1800" windowWidth="20700" windowHeight="11565" xr2:uid="{CBC5439E-15C6-4517-9685-D3D022368B88}"/>
+    <workbookView xWindow="-28920" yWindow="-2790" windowWidth="29040" windowHeight="16080" xr2:uid="{52CFF134-1097-4993-A9A6-09D50BC5AF3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,30 +118,43 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -171,18 +184,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -498,1078 +515,1312 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F93A9C8-AAAE-410F-9741-BC809576A708}">
-  <dimension ref="A1:M26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC94E85-52C2-46DF-89C2-FD5D543C0F8B}">
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M26"/>
+      <selection sqref="A1:P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="90.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>22120044</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2">
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3">
         <v>3.05</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="3">
         <v>2.85</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="3">
         <v>2.8</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="3">
         <v>2.78</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="I1" s="4">
+        <v>2.82</v>
+      </c>
+      <c r="J1" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="K1" s="5">
         <v>2.5</v>
       </c>
-      <c r="I1" s="3">
+      <c r="L1" s="5">
         <v>3.5</v>
       </c>
-      <c r="J1" s="4">
-        <v>0</v>
-      </c>
-      <c r="K1" s="3">
+      <c r="M1" s="6">
+        <v>0</v>
+      </c>
+      <c r="N1" s="5">
         <v>2.5</v>
       </c>
-      <c r="L1" s="4">
-        <v>0</v>
-      </c>
-      <c r="M1" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+      <c r="O1" s="6">
+        <v>0</v>
+      </c>
+      <c r="P1" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>22120045</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
         <v>0.68</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>0.44</v>
       </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
         <v>1.5</v>
       </c>
-      <c r="H2" s="3">
-        <v>0</v>
+      <c r="H2" s="4">
+        <v>1.6</v>
       </c>
       <c r="I2" s="4">
-        <v>0</v>
+        <v>1.64</v>
       </c>
       <c r="J2" s="4">
-        <v>0</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0</v>
-      </c>
-      <c r="L2" s="4">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>1.7</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0</v>
+      </c>
+      <c r="O2" s="6">
+        <v>0</v>
+      </c>
+      <c r="P2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>22120046</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
         <v>1.98</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>2.4900000000000002</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>2.63</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <v>2.82</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="4">
+        <v>2.85</v>
+      </c>
+      <c r="I3" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="J3" s="4">
+        <v>2.94</v>
+      </c>
+      <c r="K3" s="5">
         <v>2.5</v>
       </c>
-      <c r="I3" s="3">
+      <c r="L3" s="5">
         <v>3.5</v>
       </c>
-      <c r="J3" s="4">
-        <v>0</v>
-      </c>
-      <c r="K3" s="3">
+      <c r="M3" s="6">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
         <v>2.5</v>
       </c>
-      <c r="L3" s="4">
-        <v>0</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+      <c r="O3" s="6">
+        <v>0</v>
+      </c>
+      <c r="P3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>22120047</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
         <v>0.64</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>0.75</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>0.85</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <v>0.9</v>
       </c>
       <c r="H4" s="4">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I4" s="4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="6">
+        <v>0</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>22120048</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
         <v>1.23</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>1.3</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <v>1.5</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <v>1.7</v>
       </c>
       <c r="H5" s="4">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="I5" s="4">
-        <v>0</v>
+        <v>1.86</v>
       </c>
       <c r="J5" s="4">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0</v>
-      </c>
-      <c r="L5" s="4">
-        <v>0</v>
-      </c>
-      <c r="M5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>1.9</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0</v>
+      </c>
+      <c r="O5" s="6">
+        <v>0</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="90.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>22120049</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
         <v>3.11</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>1.64</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <v>1.9</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="3">
         <v>1.95</v>
       </c>
-      <c r="H6" s="3">
-        <v>0</v>
+      <c r="H6" s="4">
+        <v>2</v>
       </c>
       <c r="I6" s="4">
-        <v>0</v>
+        <v>2.11</v>
       </c>
       <c r="J6" s="4">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0</v>
-      </c>
-      <c r="L6" s="4">
-        <v>0</v>
-      </c>
-      <c r="M6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6">
+        <v>0</v>
+      </c>
+      <c r="O6" s="6">
+        <v>0</v>
+      </c>
+      <c r="P6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>22120051</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
         <v>3.11</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>2.92</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <v>2.4900000000000002</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <v>2.38</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="J7" s="4">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="K7" s="5">
         <v>2</v>
       </c>
-      <c r="I7" s="3">
-        <v>1</v>
-      </c>
-      <c r="J7" s="3">
-        <v>1</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0</v>
-      </c>
-      <c r="L7" s="4">
-        <v>0</v>
-      </c>
-      <c r="M7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+      <c r="L7" s="5">
+        <v>1</v>
+      </c>
+      <c r="M7" s="5">
+        <v>1</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="6">
+        <v>0</v>
+      </c>
+      <c r="P7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>22120052</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
         <v>2.11</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>1.34</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="3">
         <v>1.07</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="3">
         <v>1.32</v>
       </c>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0</v>
+      <c r="H8" s="4">
+        <v>1.45</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1.65</v>
       </c>
       <c r="J8" s="4">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4">
-        <v>0</v>
-      </c>
-      <c r="L8" s="4">
-        <v>0</v>
-      </c>
-      <c r="M8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>1.75</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0</v>
+      </c>
+      <c r="N8" s="6">
+        <v>0</v>
+      </c>
+      <c r="O8" s="6">
+        <v>0</v>
+      </c>
+      <c r="P8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>22120053</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
         <v>3.14</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>2.85</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="3">
         <v>2.4700000000000002</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="3">
         <v>2.41</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="4">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="I9" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="J9" s="4">
+        <v>2.65</v>
+      </c>
+      <c r="K9" s="5">
         <v>3</v>
       </c>
-      <c r="I9" s="3">
+      <c r="L9" s="5">
         <v>2</v>
       </c>
-      <c r="J9" s="3">
-        <v>1</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4">
-        <v>0</v>
-      </c>
-      <c r="M9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+      <c r="M9" s="5">
+        <v>1</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0</v>
+      </c>
+      <c r="O9" s="6">
+        <v>0</v>
+      </c>
+      <c r="P9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>22120054</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
         <v>2.66</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>2.68</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="3">
         <v>2.27</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="3">
         <v>2.27</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="4">
+        <v>2.23</v>
+      </c>
+      <c r="I10" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J10" s="4">
+        <v>2.35</v>
+      </c>
+      <c r="K10" s="5">
         <v>3</v>
       </c>
-      <c r="I10" s="3">
+      <c r="L10" s="5">
         <v>2.5</v>
       </c>
-      <c r="J10" s="3">
-        <v>0</v>
-      </c>
-      <c r="K10" s="4">
-        <v>0</v>
-      </c>
-      <c r="L10" s="4">
-        <v>0</v>
-      </c>
-      <c r="M10" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0</v>
+      </c>
+      <c r="O10" s="6">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="90.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>22120055</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
         <v>0.32</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>0.32</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="3">
         <v>0.21</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="3">
         <v>0.35</v>
       </c>
       <c r="H11" s="4">
-        <v>0</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0</v>
+        <v>0.45</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0.5</v>
       </c>
       <c r="J11" s="4">
-        <v>0</v>
-      </c>
-      <c r="K11" s="4">
-        <v>0</v>
-      </c>
-      <c r="L11" s="4">
-        <v>0</v>
-      </c>
-      <c r="M11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>0.65</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+      <c r="M11" s="6">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0</v>
+      </c>
+      <c r="O11" s="6">
+        <v>0</v>
+      </c>
+      <c r="P11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>22120056</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>2</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="3">
         <v>3.14</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="3">
         <v>3.01</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="3">
         <v>2.77</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="3">
         <v>2.83</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="4">
+        <v>2.85</v>
+      </c>
+      <c r="I12" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="J12" s="4">
+        <v>3</v>
+      </c>
+      <c r="K12" s="5">
         <v>2.5</v>
       </c>
-      <c r="I12" s="3">
+      <c r="L12" s="5">
         <v>2</v>
       </c>
-      <c r="J12" s="3">
+      <c r="M12" s="5">
         <v>2.5</v>
       </c>
-      <c r="K12" s="3">
-        <v>1</v>
-      </c>
-      <c r="L12" s="4">
-        <v>0</v>
-      </c>
-      <c r="M12" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="N12" s="5">
+        <v>1</v>
+      </c>
+      <c r="O12" s="6">
+        <v>0</v>
+      </c>
+      <c r="P12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="105.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>22120057</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
         <v>2.64</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="3">
         <v>2.9</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="3">
         <v>2.5499999999999998</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="3">
         <v>2.2200000000000002</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="I13" s="4">
+        <v>2.35</v>
+      </c>
+      <c r="J13" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="K13" s="5">
         <v>2</v>
       </c>
-      <c r="I13" s="3">
+      <c r="L13" s="5">
         <v>2.5</v>
       </c>
-      <c r="J13" s="3">
-        <v>0</v>
-      </c>
-      <c r="K13" s="4">
-        <v>0</v>
-      </c>
-      <c r="L13" s="4">
-        <v>0</v>
-      </c>
-      <c r="M13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+      <c r="N13" s="6">
+        <v>0</v>
+      </c>
+      <c r="O13" s="6">
+        <v>0</v>
+      </c>
+      <c r="P13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="90.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>22120058</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <v>2</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="3">
         <v>2.98</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="3">
         <v>2.93</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="3">
         <v>2.76</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="3">
         <v>2.76</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="I14" s="4">
+        <v>2.86</v>
+      </c>
+      <c r="J14" s="4">
+        <v>3</v>
+      </c>
+      <c r="K14" s="5">
         <v>2.5</v>
       </c>
-      <c r="I14" s="3">
+      <c r="L14" s="5">
         <v>2</v>
       </c>
-      <c r="J14" s="3">
+      <c r="M14" s="5">
         <v>2</v>
       </c>
-      <c r="K14" s="3">
+      <c r="N14" s="5">
         <v>2.5</v>
       </c>
-      <c r="L14" s="4">
-        <v>0</v>
-      </c>
-      <c r="M14" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
+      <c r="O14" s="6">
+        <v>0</v>
+      </c>
+      <c r="P14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>22120059</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>2</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="3">
         <v>1.59</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="3">
         <v>1.36</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="3">
         <v>1.39</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="3">
         <v>1.68</v>
       </c>
-      <c r="H15" s="3">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3">
+      <c r="H15" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1.76</v>
+      </c>
+      <c r="J15" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0</v>
+      </c>
+      <c r="L15" s="5">
         <v>3.75</v>
       </c>
-      <c r="J15" s="4">
-        <v>0</v>
-      </c>
-      <c r="K15" s="4">
-        <v>0</v>
-      </c>
-      <c r="L15" s="4">
-        <v>0</v>
-      </c>
-      <c r="M15" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="M15" s="6">
+        <v>0</v>
+      </c>
+      <c r="N15" s="6">
+        <v>0</v>
+      </c>
+      <c r="O15" s="6">
+        <v>0</v>
+      </c>
+      <c r="P15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>22120060</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
         <v>0.91</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="3">
         <v>0.59</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="3">
         <v>0.6</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="3">
         <v>0.9</v>
       </c>
-      <c r="H16" s="3">
-        <v>0</v>
+      <c r="H16" s="4">
+        <v>0.95</v>
       </c>
       <c r="I16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="4">
-        <v>0</v>
-      </c>
-      <c r="K16" s="4">
-        <v>0</v>
-      </c>
-      <c r="L16" s="4">
-        <v>0</v>
-      </c>
-      <c r="M16" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+        <v>1.25</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6">
+        <v>0</v>
+      </c>
+      <c r="M16" s="6">
+        <v>0</v>
+      </c>
+      <c r="N16" s="6">
+        <v>0</v>
+      </c>
+      <c r="O16" s="6">
+        <v>0</v>
+      </c>
+      <c r="P16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>22120061</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
         <v>2.86</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="3">
         <v>2.95</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="3">
         <v>2.94</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="3">
         <v>3.01</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="4">
+        <v>3.06</v>
+      </c>
+      <c r="I17" s="4">
+        <v>3.11</v>
+      </c>
+      <c r="J17" s="4">
+        <v>3.34</v>
+      </c>
+      <c r="K17" s="5">
         <v>2.5</v>
       </c>
-      <c r="I17" s="3">
+      <c r="L17" s="5">
         <v>3.5</v>
       </c>
-      <c r="J17" s="3">
+      <c r="M17" s="5">
         <v>3</v>
       </c>
-      <c r="K17" s="3">
+      <c r="N17" s="5">
         <v>2.5</v>
       </c>
-      <c r="L17" s="4">
-        <v>0</v>
-      </c>
-      <c r="M17" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+      <c r="O17" s="6">
+        <v>0</v>
+      </c>
+      <c r="P17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>22120062</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <v>2</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="3">
         <v>3.16</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="3">
         <v>3.23</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="3">
         <v>3.17</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="3">
         <v>3.05</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="4">
+        <v>3.11</v>
+      </c>
+      <c r="I18" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="J18" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="K18" s="5">
         <v>3.5</v>
       </c>
-      <c r="I18" s="3">
+      <c r="L18" s="5">
         <v>2.5</v>
       </c>
-      <c r="J18" s="3">
+      <c r="M18" s="5">
         <v>2</v>
       </c>
-      <c r="K18" s="3">
+      <c r="N18" s="5">
         <v>2</v>
       </c>
-      <c r="L18" s="4">
-        <v>0</v>
-      </c>
-      <c r="M18" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="24" x14ac:dyDescent="0.25">
+      <c r="O18" s="6">
+        <v>0</v>
+      </c>
+      <c r="P18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>22120063</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2">
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
         <v>2.7</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="3">
         <v>2.81</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="3">
         <v>2.65</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="3">
         <v>2.38</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="I19" s="4">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="J19" s="4">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="K19" s="5">
         <v>2.5</v>
       </c>
-      <c r="I19" s="3">
+      <c r="L19" s="5">
         <v>2</v>
       </c>
-      <c r="J19" s="3">
-        <v>0</v>
-      </c>
-      <c r="K19" s="3">
+      <c r="M19" s="5">
+        <v>0</v>
+      </c>
+      <c r="N19" s="5">
         <v>2</v>
       </c>
-      <c r="L19" s="4">
-        <v>0</v>
-      </c>
-      <c r="M19" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="24" x14ac:dyDescent="0.25">
+      <c r="O19" s="6">
+        <v>0</v>
+      </c>
+      <c r="P19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>22120064</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
         <v>3.18</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="3">
         <v>3.24</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="3">
         <v>3.24</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="3">
         <v>3.18</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="I20" s="4">
+        <v>3.25</v>
+      </c>
+      <c r="J20" s="4">
+        <v>3.45</v>
+      </c>
+      <c r="K20" s="5">
         <v>3</v>
       </c>
-      <c r="I20" s="3">
+      <c r="L20" s="5">
         <v>3.75</v>
       </c>
-      <c r="J20" s="3">
+      <c r="M20" s="5">
         <v>3.5</v>
       </c>
-      <c r="K20" s="3">
+      <c r="N20" s="5">
         <v>3</v>
       </c>
-      <c r="L20" s="4">
-        <v>0</v>
-      </c>
-      <c r="M20" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="O20" s="6">
+        <v>0</v>
+      </c>
+      <c r="P20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="90.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>22120065</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2">
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
         <v>1.32</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="3">
         <v>1.25</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="3">
         <v>1.5</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="3">
         <v>1.7</v>
       </c>
       <c r="H21" s="4">
-        <v>0</v>
+        <v>1.33</v>
       </c>
       <c r="I21" s="4">
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="J21" s="4">
-        <v>0</v>
-      </c>
-      <c r="K21" s="4">
-        <v>0</v>
-      </c>
-      <c r="L21" s="4">
-        <v>0</v>
-      </c>
-      <c r="M21" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+        <v>1.8</v>
+      </c>
+      <c r="K21" s="6">
+        <v>0</v>
+      </c>
+      <c r="L21" s="6">
+        <v>0</v>
+      </c>
+      <c r="M21" s="6">
+        <v>0</v>
+      </c>
+      <c r="N21" s="6">
+        <v>0</v>
+      </c>
+      <c r="O21" s="6">
+        <v>0</v>
+      </c>
+      <c r="P21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>22120066</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2">
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
         <v>2.11</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="3">
         <v>1.88</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="3">
         <v>1.46</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="3">
         <v>1.2</v>
       </c>
-      <c r="H22" s="3">
-        <v>1</v>
-      </c>
-      <c r="I22" s="3">
-        <v>0</v>
-      </c>
-      <c r="J22" s="3">
-        <v>0</v>
-      </c>
-      <c r="K22" s="3">
-        <v>0</v>
-      </c>
-      <c r="L22" s="3">
-        <v>0</v>
-      </c>
-      <c r="M22" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="35.25" x14ac:dyDescent="0.25">
+      <c r="H22" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J22" s="4">
+        <v>1.56</v>
+      </c>
+      <c r="K22" s="5">
+        <v>1</v>
+      </c>
+      <c r="L22" s="5">
+        <v>0</v>
+      </c>
+      <c r="M22" s="5">
+        <v>0</v>
+      </c>
+      <c r="N22" s="5">
+        <v>0</v>
+      </c>
+      <c r="O22" s="5">
+        <v>0</v>
+      </c>
+      <c r="P22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22120067</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2">
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
         <v>2.98</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="3">
         <v>3.05</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="3">
         <v>2.67</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="3">
         <v>2.58</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="4">
+        <v>2.58</v>
+      </c>
+      <c r="I23" s="4">
+        <v>2.65</v>
+      </c>
+      <c r="J23" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="K23" s="5">
         <v>3</v>
       </c>
-      <c r="I23" s="3">
-        <v>0</v>
-      </c>
-      <c r="J23" s="3">
+      <c r="L23" s="5">
+        <v>0</v>
+      </c>
+      <c r="M23" s="5">
         <v>2</v>
       </c>
-      <c r="K23" s="4">
-        <v>0</v>
-      </c>
-      <c r="L23" s="4">
-        <v>0</v>
-      </c>
-      <c r="M23" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="N23" s="6">
+        <v>0</v>
+      </c>
+      <c r="O23" s="6">
+        <v>0</v>
+      </c>
+      <c r="P23" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22120068</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2">
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3">
         <v>3.25</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="3">
         <v>3.21</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="3">
         <v>3.02</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="3">
         <v>3</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="4">
+        <v>3</v>
+      </c>
+      <c r="I24" s="4">
+        <v>3.11</v>
+      </c>
+      <c r="J24" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="K24" s="5">
         <v>2.5</v>
       </c>
-      <c r="I24" s="3">
+      <c r="L24" s="5">
         <v>3.75</v>
       </c>
-      <c r="J24" s="3">
+      <c r="M24" s="5">
         <v>3</v>
       </c>
-      <c r="K24" s="3">
-        <v>0</v>
-      </c>
-      <c r="L24" s="4">
-        <v>0</v>
-      </c>
-      <c r="M24" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="24" x14ac:dyDescent="0.25">
+      <c r="N24" s="5">
+        <v>0</v>
+      </c>
+      <c r="O24" s="6">
+        <v>0</v>
+      </c>
+      <c r="P24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22120069</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2">
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3">
         <v>2.4300000000000002</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="3">
         <v>2.46</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="3">
         <v>2.2400000000000002</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="I25" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J25" s="4">
+        <v>2.33</v>
+      </c>
+      <c r="K25" s="5">
         <v>2.5</v>
       </c>
-      <c r="I25" s="3">
+      <c r="L25" s="5">
         <v>3.5</v>
       </c>
-      <c r="J25" s="4">
-        <v>0</v>
-      </c>
-      <c r="K25" s="3">
-        <v>0</v>
-      </c>
-      <c r="L25" s="4">
-        <v>0</v>
-      </c>
-      <c r="M25" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="57.75" x14ac:dyDescent="0.25">
+      <c r="M25" s="6">
+        <v>0</v>
+      </c>
+      <c r="N25" s="5">
+        <v>0</v>
+      </c>
+      <c r="O25" s="6">
+        <v>0</v>
+      </c>
+      <c r="P25" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="90.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22120070</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="D26" s="2">
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3">
         <v>2.4300000000000002</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="3">
         <v>2.2799999999999998</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="3">
         <v>2.2599999999999998</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="3">
         <v>2.0499999999999998</v>
       </c>
-      <c r="H26" s="3">
-        <v>0</v>
-      </c>
-      <c r="I26" s="3">
-        <v>1</v>
-      </c>
-      <c r="J26" s="3">
-        <v>0</v>
-      </c>
-      <c r="K26" s="3">
+      <c r="H26" s="4">
+        <v>2.08</v>
+      </c>
+      <c r="I26" s="4">
+        <v>2.12</v>
+      </c>
+      <c r="J26" s="4">
+        <v>2.14</v>
+      </c>
+      <c r="K26" s="5">
+        <v>0</v>
+      </c>
+      <c r="L26" s="5">
+        <v>1</v>
+      </c>
+      <c r="M26" s="5">
+        <v>0</v>
+      </c>
+      <c r="N26" s="5">
         <v>3</v>
       </c>
-      <c r="L26" s="4">
-        <v>0</v>
-      </c>
-      <c r="M26" s="4">
+      <c r="O26" s="6">
+        <v>0</v>
+      </c>
+      <c r="P26" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>